<commit_message>
Include decorator module in setup
Decorated functions in early versions of Python struggle to propagate
their signatures up to the decorators, according to the module inspect.
The third-party decorator module wraps up a solution to this problem, so
is now included in the Optima Core module setup file.
</commit_message>
<xml_diff>
--- a/tests/frameworks/cascade-minimal.xlsx
+++ b/tests/frameworks/cascade-minimal.xlsx
@@ -2578,9 +2578,6 @@
     <t>Population Type B</t>
   </si>
   <si>
-    <t>Population Type</t>
-  </si>
-  <si>
     <t>Source for Population Existence Commencement (Type A)</t>
   </si>
   <si>
@@ -2663,6 +2660,9 @@
   </si>
   <si>
     <t>Cascade Plot Option</t>
+  </si>
+  <si>
+    <t>Population Types</t>
   </si>
 </sst>
 </file>
@@ -3660,14 +3660,14 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.3984375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.06640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.9296875" style="2" bestFit="1" customWidth="1"/>
@@ -3684,33 +3684,33 @@
         <v>767</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>770</v>
+        <v>798</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>793</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>794</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>795</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>796</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>797</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="26" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C2" t="s">
         <v>764</v>
@@ -3721,10 +3721,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="26" t="s">
+        <v>772</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>773</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>774</v>
       </c>
       <c r="C3" t="s">
         <v>764</v>
@@ -3735,10 +3735,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>775</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>776</v>
       </c>
       <c r="C4" t="s">
         <v>764</v>
@@ -3749,10 +3749,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="26" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C5" t="s">
         <v>764</v>
@@ -3763,10 +3763,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="26" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C6" t="s">
         <v>764</v>
@@ -3774,10 +3774,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="26" t="s">
+        <v>777</v>
+      </c>
+      <c r="B7" s="26" t="s">
         <v>778</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>779</v>
       </c>
       <c r="C7" t="s">
         <v>764</v>
@@ -3785,10 +3785,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C8" t="s">
         <v>765</v>
@@ -3799,10 +3799,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="26" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C9" t="s">
         <v>765</v>
@@ -3813,10 +3813,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="26" t="s">
+        <v>783</v>
+      </c>
+      <c r="B10" s="26" t="s">
         <v>784</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>785</v>
       </c>
       <c r="C10" t="s">
         <v>765</v>
@@ -3827,10 +3827,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="26" t="s">
+        <v>785</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>786</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>787</v>
       </c>
       <c r="C11" t="s">
         <v>765</v>
@@ -3838,10 +3838,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="26" t="s">
+        <v>787</v>
+      </c>
+      <c r="B12" s="26" t="s">
         <v>788</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>789</v>
       </c>
       <c r="C12" t="s">
         <v>765</v>
@@ -3990,52 +3990,52 @@
         <v>768</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>771</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>772</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>773</v>
-      </c>
       <c r="D1" s="26" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="26" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="26" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="26" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="26" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="26" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="26" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -4043,44 +4043,44 @@
         <v>769</v>
       </c>
       <c r="B9" s="26" t="s">
+        <v>779</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>780</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>781</v>
-      </c>
       <c r="D9" s="26" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="26" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="26" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="26" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="26" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>